<commit_message>
back engineering of stage and jam factor tables for RF
</commit_message>
<xml_diff>
--- a/jra/pyplot_way/calculations.xlsx
+++ b/jra/pyplot_way/calculations.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7440"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="43">
   <si>
     <t xml:space="preserve">The location of the platform at the two first waypoints are </t>
   </si>
@@ -139,6 +139,12 @@
   </si>
   <si>
     <t>s</t>
+  </si>
+  <si>
+    <t>and as such, the elevation and azimuth angles at for threats 1 and 2 are</t>
+  </si>
+  <si>
+    <t>elevation</t>
   </si>
 </sst>
 </file>
@@ -484,10 +490,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:U55"/>
+  <dimension ref="A2:U59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="M55" sqref="M55"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -590,7 +596,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -607,15 +613,15 @@
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B17" s="1">
         <f>B5+(B14/2)*B10</f>
-        <v>0.88888888888888884</v>
+        <v>0.44444444444444442</v>
       </c>
       <c r="C17" s="1">
         <f>C5+(B14/2)*C10</f>
-        <v>3.3333333333333335</v>
+        <v>3.1666666666666665</v>
       </c>
       <c r="D17" s="1">
         <f>D5+(B14/2)*D10</f>
-        <v>13.333333333333334</v>
+        <v>13.666666666666666</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
@@ -983,15 +989,15 @@
       </c>
       <c r="C45" s="1">
         <f>B35-B17</f>
-        <v>6.1111111111111107</v>
+        <v>6.5555555555555554</v>
       </c>
       <c r="D45" s="1">
         <f>C35-C17</f>
-        <v>1.6666666666666665</v>
+        <v>1.8333333333333335</v>
       </c>
       <c r="E45" s="1">
         <f>D35-D17</f>
-        <v>-13.333333333333334</v>
+        <v>-13.666666666666666</v>
       </c>
     </row>
     <row r="46" spans="1:21" x14ac:dyDescent="0.25">
@@ -1000,15 +1006,15 @@
       </c>
       <c r="C46" s="1">
         <f>B36-B17</f>
-        <v>5.1111111111111107</v>
+        <v>5.5555555555555554</v>
       </c>
       <c r="D46" s="1">
         <f>C36-C17</f>
-        <v>2.6666666666666665</v>
+        <v>2.8333333333333335</v>
       </c>
       <c r="E46" s="1">
         <f>D36-D17</f>
-        <v>-13.333333333333334</v>
+        <v>-13.666666666666666</v>
       </c>
     </row>
     <row r="48" spans="1:21" x14ac:dyDescent="0.25">
@@ -1016,12 +1022,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="49" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="J49" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="50" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C50" s="1" t="s">
         <v>16</v>
       </c>
@@ -1041,21 +1047,21 @@
         <v>18</v>
       </c>
     </row>
-    <row r="51" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B51" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C51" s="1">
         <f>S38*C45+T38*D45+U38*E45</f>
-        <v>5.2679120192840596</v>
+        <v>5.6669930498496459</v>
       </c>
       <c r="D51" s="1">
         <f>S39*C45+T39*D45+U39*E45</f>
-        <v>-0.19546622695703686</v>
+        <v>-0.16712153539168262</v>
       </c>
       <c r="E51" s="1">
         <f>C45*S40+D45*T40+E45*U40</f>
-        <v>-10.911561824390795</v>
+        <v>-11.184350870000564</v>
       </c>
       <c r="J51" s="1">
         <v>2</v>
@@ -1075,21 +1081,21 @@
         <v>37</v>
       </c>
     </row>
-    <row r="52" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B52" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C52" s="1">
         <f>C46*S38+D46*T38+U38*E46</f>
-        <v>4.8527744326955302</v>
+        <v>5.2518554632611165</v>
       </c>
       <c r="D52" s="1">
         <f>C46*S39+D46*T39+E46*U39</f>
-        <v>1.0282108361783531</v>
+        <v>1.0565555277437073</v>
       </c>
       <c r="E52" s="1">
         <f>C46*S40+D46*T40+E46*U40</f>
-        <v>-10.911561824390795</v>
+        <v>-11.184350870000564</v>
       </c>
       <c r="K52" s="1">
         <v>5.2518599999999998</v>
@@ -1105,7 +1111,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="53" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="J53" s="1">
         <v>4</v>
       </c>
@@ -1123,7 +1129,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="54" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="K54" s="1">
         <v>4.8527699999999996</v>
       </c>
@@ -1138,9 +1144,23 @@
         <v>38</v>
       </c>
     </row>
-    <row r="55" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M55" s="1" t="s">
         <v>40</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B59" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C59" s="1" t="e">
+        <f>ASIN((M51-D17)/(SQRT((K51-B17)^2+(L51-C17)^2+(-D17)^2)))</f>
+        <v>#NUM!</v>
       </c>
     </row>
   </sheetData>

</xml_diff>